<commit_message>
Code run throught parameter DDT 003
</commit_message>
<xml_diff>
--- a/TestData/Test_Data.xlsx
+++ b/TestData/Test_Data.xlsx
@@ -9,7 +9,7 @@
     <sheet name="CredKart_login_Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -393,7 +393,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D2" sqref="D2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>

</xml_diff>